<commit_message>
Fixed a lot of errors introduced by previous commit
</commit_message>
<xml_diff>
--- a/2D_Framework/Base/Image/MapDesign.xlsx
+++ b/2D_Framework/Base/Image/MapDesign.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KahWei\Git\Game-Dev\2D_Framework\Base\Image\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035"/>
   </bookViews>
@@ -82,11 +87,25 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -135,7 +154,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -170,7 +189,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -381,8 +400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2221,13 +2240,13 @@
         <v>0</v>
       </c>
       <c r="D19" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E19" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F19" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="G19" s="2">
         <v>0</v>
@@ -2918,6 +2937,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:AG25">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>